<commit_message>
feat: organizing output structure and result file
</commit_message>
<xml_diff>
--- a/backend/apps/extractor/exporter/export_template.xlsx
+++ b/backend/apps/extractor/exporter/export_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isabella\dev\llms\isabella\extractor\exporter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabella/dev/ragify-app/backend/apps/extractor/exporter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F20510C-7E76-4C0E-8A75-0E8359C5167A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2876DC-D8D7-1A40-8F97-AE98261D4EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99B4DB9F-F710-45A8-9B63-A0EB0325E7B4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{99B4DB9F-F710-45A8-9B63-A0EB0325E7B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Resultado" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>PROMPT</t>
   </si>
   <si>
-    <t>ID PROMPT</t>
-  </si>
-  <si>
     <t>RESULTADO</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>Retriever encontrou resposta?</t>
+  </si>
+  <si>
+    <t>VARIÁVEL</t>
   </si>
 </sst>
 </file>
@@ -489,6 +489,9 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -542,9 +545,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -873,23 +873,23 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="8"/>
-    <col min="2" max="2" width="20.42578125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="8"/>
-    <col min="4" max="9" width="15.7109375" style="12"/>
-    <col min="10" max="11" width="15.7109375" style="13"/>
-    <col min="12" max="12" width="15.7109375" style="12"/>
+    <col min="1" max="1" width="15.6640625" style="8"/>
+    <col min="2" max="2" width="20.5" style="25" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="8"/>
+    <col min="4" max="9" width="15.6640625" style="12"/>
+    <col min="10" max="11" width="15.6640625" style="13"/>
+    <col min="12" max="12" width="15.6640625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
@@ -899,24 +899,24 @@
       <c r="K1"/>
       <c r="L1"/>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-    </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+    </row>
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>21</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="47" t="s">
-        <v>22</v>
+      <c r="D3" s="29" t="s">
+        <v>21</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -927,7 +927,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -935,7 +935,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
@@ -943,7 +943,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -954,7 +954,7 @@
       <c r="K6"/>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -965,7 +965,7 @@
       <c r="K7"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -976,7 +976,7 @@
       <c r="K8"/>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -987,7 +987,7 @@
       <c r="K9"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -998,7 +998,7 @@
       <c r="K10"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
       <c r="J11" s="12"/>
@@ -1022,34 +1022,34 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="4" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="27" customWidth="1"/>
-    <col min="4" max="7" width="20.7109375" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="20.7109375" style="4"/>
+    <col min="1" max="1" width="20.6640625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="27" customWidth="1"/>
+    <col min="4" max="7" width="20.6640625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="20.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-    </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+    </row>
+    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="38"/>
-    </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
+    </row>
+    <row r="3" spans="1:5" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="35"/>
       <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
@@ -1060,14 +1060,14 @@
         <v>3</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
     </row>
@@ -1090,42 +1090,42 @@
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.6640625" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="6" width="25.7109375" style="14"/>
+    <col min="5" max="6" width="25.6640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="46"/>
-    </row>
-    <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="47"/>
+    </row>
+    <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="39" t="s">
+      <c r="B2" s="44"/>
+      <c r="C2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="39" t="s">
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="41"/>
-    </row>
-    <row r="3" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="42"/>
+    </row>
+    <row r="3" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>6</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>

</xml_diff>